<commit_message>
Filtrado y pegado de datos
</commit_message>
<xml_diff>
--- a/Data/Output/Alejandra_datos.xlsx
+++ b/Data/Output/Alejandra_datos.xlsx
@@ -491,15 +491,27 @@
           <t xml:space="preserve">11012024 </t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ALEJANDRA S FASHIÓON INC</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>35,783.00</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>5293</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Settlement Date no encontrado</t>
+          <t>2024-11-08</t>
         </is>
       </c>
     </row>

</xml_diff>